<commit_message>
Typesetting of Chapters 0-2
</commit_message>
<xml_diff>
--- a/1.0 - Introduction/assets/tables/UR - 1.0 - table_1.xlsx
+++ b/1.0 - Introduction/assets/tables/UR - 1.0 - table_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38380" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Product</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Scale</t>
   </si>
   <si>
-    <t>Data requirements</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>To inform design of building-level/asset-level risk reduction activities and promote avoidance of new risk</t>
   </si>
   <si>
-    <t>Building/</t>
-  </si>
-  <si>
-    <t>infrastructure level</t>
-  </si>
-  <si>
     <t xml:space="preserve">Moderate-high: Requires high-resolution local data for large spatial areas with clear articulation </t>
   </si>
   <si>
@@ -127,13 +118,19 @@
   </si>
   <si>
     <t>High: Requires high-resolution, high-quality data of uncertainty</t>
+  </si>
+  <si>
+    <t>Building / infrastructure level</t>
+  </si>
+  <si>
+    <t>Data Requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,13 +144,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Verb Light"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Verb Semibold"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A818F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,21 +194,377 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7EAED"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4A818F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Verb Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Verb Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Verb Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Verb Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Verb Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Verb Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="0"/>
+        <name val="Verb Semibold"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4A818F"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7EAED"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4A818F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="medium">
+          <color rgb="FF4A818F"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF4A818F"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF4A818F"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF4A818F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7EAED"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4A818F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF2F2F2F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thick">
+          <color rgb="FF989A9D"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF989A9D"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF989A9D"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF989A9D"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="3" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="GAR Table" pivot="0" count="4">
+      <tableStyleElement type="wholeTable" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+    </tableStyle>
+    <tableStyle name="GAR Table Final" pivot="0" count="4">
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+    </tableStyle>
+    <tableStyle name="GAR Table Final 2" pivot="0" count="4">
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:E8"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Product" dataDxfId="8"/>
+    <tableColumn id="2" name="Purpose" dataDxfId="7"/>
+    <tableColumn id="3" name="Scale" dataDxfId="6"/>
+    <tableColumn id="4" name="Data Requirements" dataDxfId="5"/>
+    <tableColumn id="5" name="Cost" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="GAR Table Final 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -504,165 +889,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="21.25" style="1" customWidth="1"/>
+    <col min="1" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="24" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="50" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="48">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:5" ht="50" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="50" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="48">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
+    <row r="5" spans="1:5" ht="50" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="48">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
+    <row r="6" spans="1:5" ht="50" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="80">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
+    <row r="7" spans="1:5" ht="50" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="64">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="48">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:5" ht="50" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="80">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="80">
-      <c r="A9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>